<commit_message>
Update Sara Contact Info & Jurisdiction
</commit_message>
<xml_diff>
--- a/DefinitionInformationTable.xlsx
+++ b/DefinitionInformationTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\EPI\Syndromic Surveillance\R Code\DefinitionComparison\TwoDefinitions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TJB0303\LocalSave\R\GitHub\syndrome-definition-evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6EC3429-D67C-4E99-AFF6-417E650B51D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9962A27-7F12-48CF-9D98-740EDE5B2E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D30C9C86-3D98-4204-9FB5-C398A54A23E4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D30C9C86-3D98-4204-9FB5-C398A54A23E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="5" r:id="rId1"/>
@@ -88,9 +88,6 @@
     <t>[The jurisdiction you are applying this query to.]</t>
   </si>
   <si>
-    <t>Maricopa County, AZ</t>
-  </si>
-  <si>
     <t>Field</t>
   </si>
   <si>
@@ -139,9 +136,6 @@
     <t>[Your organization name.]</t>
   </si>
   <si>
-    <t>Maricopa County Department of Public Health</t>
-  </si>
-  <si>
     <t>[Enter the fields that you want to use to explore in more detail. For each field listed below, you will see a "Top 5" chart showing the top 5 most qrequnetly occuring free-text terms in that field. You must use the name as listed in the NSSP Data Dictionary "ESSENCE API and Data Details" tab under the "Data Details Web Display Name" column</t>
   </si>
   <si>
@@ -193,9 +187,6 @@
     <t>https://essence.syndromicsurveillance.org/nssp_essence/api/dataDetails/csv?endDate=20Jul2021&amp;geography=az_maricopa&amp;percentParam=noPercent&amp;datasource=va_hosp&amp;startDate=21Apr2021&amp;medicalGroupingSystem=essencesyndromes&amp;userId=1555&amp;aqtTarget=DataDetails&amp;ccddCategory=cdc%20anxiety%20disorders%20v1&amp;geographySystem=hospitalregion&amp;detector=probrepswitch&amp;timeResolution=daily</t>
   </si>
   <si>
-    <t>sara.chronister@maricopa.gov</t>
-  </si>
-  <si>
     <t>[Your email address.]</t>
   </si>
   <si>
@@ -209,6 +200,15 @@
   </si>
   <si>
     <t>Asthma-related visits</t>
+  </si>
+  <si>
+    <t>Washington State</t>
+  </si>
+  <si>
+    <t>Washington State Department of Health</t>
+  </si>
+  <si>
+    <t>Sara.Chronnister@doh.wa.gov</t>
   </si>
 </sst>
 </file>
@@ -253,7 +253,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -263,9 +263,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -592,39 +589,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4B277CF-9876-4850-BAAE-A2FD71D015E1}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:6" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -635,33 +632,33 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>44256</v>
+      </c>
+      <c r="B3" s="4">
+        <v>44348</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
         <v>30</v>
       </c>
-      <c r="E2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
-        <v>44256</v>
-      </c>
-      <c r="B3" s="5">
-        <v>44348</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>52</v>
+      <c r="E3" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -680,65 +677,65 @@
       <selection activeCell="A3" sqref="A3:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="40.77734375" customWidth="1"/>
+    <col min="1" max="2" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -750,46 +747,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74ABFDD0-4573-4CDB-A01F-D30B440CEE7C}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="5" width="30.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="75.77734375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="75.77734375" customWidth="1"/>
+    <col min="2" max="5" width="30.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="75.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="75.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="86.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -805,73 +802,73 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="255" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="210" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>44</v>
+        <v>54</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change manual review to validation review
</commit_message>
<xml_diff>
--- a/DefinitionInformationTable.xlsx
+++ b/DefinitionInformationTable.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TJB0303\LocalSave\R\GitHub\syndrome-definition-evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E821046C-A1F5-41D2-9A28-8AA960DBF13C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AAA4F4-0D3D-4195-9E45-BFB7AF0DAEEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{D30C9C86-3D98-4204-9FB5-C398A54A23E4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D30C9C86-3D98-4204-9FB5-C398A54A23E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="5" r:id="rId1"/>
     <sheet name="AppliedFields" sheetId="6" r:id="rId2"/>
     <sheet name="DefinitionInformation" sheetId="1" r:id="rId3"/>
-    <sheet name="ManualReviewInformation" sheetId="7" r:id="rId4"/>
+    <sheet name="ValidationReviewInformation" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="85">
   <si>
     <t>Syndrome</t>
   </si>
@@ -191,12 +191,41 @@
     <t>Asthma-related visits</t>
   </si>
   <si>
-    <t>ManualReview</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">[Include Manual Review Validation.]
-If </t>
+    <t>[Review scale - LOW.]</t>
+  </si>
+  <si>
+    <t>[Review scale - HIGH.]</t>
+  </si>
+  <si>
+    <t>StratifiedSample</t>
+  </si>
+  <si>
+    <t>StratifiedVariables</t>
+  </si>
+  <si>
+    <t>ReviewScaleLow</t>
+  </si>
+  <si>
+    <t>ReviewScaleHigh</t>
+  </si>
+  <si>
+    <t>[Your reviewer ID  #.]</t>
+  </si>
+  <si>
+    <t>ReviewerID</t>
+  </si>
+  <si>
+    <t>ReviewerName</t>
+  </si>
+  <si>
+    <t>Tyler Bonnell</t>
+  </si>
+  <si>
+    <t>Lauren Draftz</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[Stratified random sample? </t>
     </r>
     <r>
       <rPr>
@@ -207,124 +236,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>TRUE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> edit "ManualReviewInformation" sheet, if </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>FALSE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> do not edit "ManualReviewInformation". </t>
-    </r>
-  </si>
-  <si>
-    <t>[Review scale - LOW.]</t>
-  </si>
-  <si>
-    <t>[Review scale - HIGH.]</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Note:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 3 options for Review scale:
-- 0-1 (0: False Positive, 1: True Positive) 
-- 1-4 (1: Very Unlikely, 2: Unlikely, 3: Likely, 4: Very Likely) 
-- 1-5 (1: Very Unlikely, 2: Unlikely, 3: Uncertain, 4: Likely, 5: Very Likely)</t>
-    </r>
-  </si>
-  <si>
-    <t>StratifiedSample</t>
-  </si>
-  <si>
-    <t>StratifiedVariables</t>
-  </si>
-  <si>
-    <t>ReviewScaleLow</t>
-  </si>
-  <si>
-    <t>ReviewScaleHigh</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>[Your reviewer ID  #.]</t>
-  </si>
-  <si>
-    <t>ReviewerID</t>
-  </si>
-  <si>
-    <t>ReviewerName</t>
-  </si>
-  <si>
-    <t>ReviewerEmail</t>
-  </si>
-  <si>
-    <t>Tyler Bonnell</t>
-  </si>
-  <si>
-    <t>Tyler.Bonnell@doh.wa.gov</t>
-  </si>
-  <si>
-    <t>Lauren Draftz</t>
-  </si>
-  <si>
-    <t>Lauren.Draftz@doh.wa.gov</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">[Stratified random sample? </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>(TRUE/FALSE)</t>
     </r>
     <r>
@@ -342,13 +253,7 @@
     <t>[Stratified random sample variable.]</t>
   </si>
   <si>
-    <t>ReviewDefinitions</t>
-  </si>
-  <si>
     <t>[Enter the fields that you want to use to explore in more detail. For each field listed below, you will see a "Top 5" chart showing the top 5 most frequently occuring free-text terms in that field. You must use the name as listed in the NSSP Data Dictionary "ESSENCE API and Data Details" tab under the "Data Details Web Display Name" column</t>
-  </si>
-  <si>
-    <t>def1,def2,def3</t>
   </si>
   <si>
     <t>https://essence.syndromicsurveillance.org/nssp_essence/api/dataDetails/csv?geography=wa&amp;datasource=va_hosp&amp;startDate=19Oct2023&amp;medicalGroupingSystem=essencesyndromes&amp;userId=4714&amp;endDate=20Oct2023&amp;percentParam=noPercent&amp;hospFacilityType=emergency%20care&amp;aqtTarget=DataDetails&amp;ccddCategory=cdc%20influenza%20dd%20v1&amp;geographySystem=hospitalstate&amp;detector=probrepswitch&amp;timeResolution=daily&amp;hasBeenE=1&amp;refValues=true</t>
@@ -521,10 +426,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">[Definition(s) to manually review.]
-</t>
-    </r>
-    <r>
       <rPr>
         <b/>
         <sz val="11"/>
@@ -533,18 +434,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Options:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 
-- A </t>
+      <t>Note:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Here's 3 recommend options for a Review Scale. You may specify a new scale with ReviewScaleLow/High as well if you want. 
+- 0-1 (0: False Positive | 1: True Positive); </t>
     </r>
     <r>
       <rPr>
@@ -555,17 +456,46 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>single</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> definiton: </t>
+      <t>Default</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- 1-3 (1: Unlikely | 2:  Uncertain | 3: Likely) 
+- 1-5 (1: Very Unlikely, 2: Unlikely | 3: Uncertain | 4: Likely, 5: Very Likely)</t>
+    </r>
+  </si>
+  <si>
+    <t>CCDDCategory_flat</t>
+  </si>
+  <si>
+    <t>Category_flat</t>
+  </si>
+  <si>
+    <t>Subcategory_flat</t>
+  </si>
+  <si>
+    <t>Procedure_Combo</t>
+  </si>
+  <si>
+    <t>DDParsed</t>
+  </si>
+  <si>
+    <t>Weekday, Month</t>
+  </si>
+  <si>
+    <t>ValidationReview</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[Include Validation Review Validation.]
+If </t>
     </r>
     <r>
       <rPr>
@@ -576,18 +506,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>def1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- </t>
+      <t>TRUE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> edit "ValidationReviewInformation" sheet, if </t>
     </r>
     <r>
       <rPr>
@@ -598,39 +527,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Multiple</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> definitions: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>def1, def2, def3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
+      <t>FALSE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do not edit "ValidationReviewInformation". </t>
     </r>
   </si>
 </sst>
@@ -1082,8 +989,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4B277CF-9876-4850-BAAE-A2FD71D015E1}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,7 +1025,7 @@
         <v>27</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -1139,7 +1048,7 @@
         <v>14</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1147,13 +1056,13 @@
         <v>30</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E3" s="6">
         <v>44256</v>
@@ -1179,7 +1088,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,7 +1098,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>34</v>
@@ -1207,25 +1116,40 @@
       <c r="A3" t="s">
         <v>25</v>
       </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1252,15 +1176,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74ABFDD0-4573-4CDB-A01F-D30B440CEE7C}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="31.7109375" style="2" customWidth="1"/>
-    <col min="4" max="5" width="30.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" style="2" customWidth="1"/>
     <col min="6" max="6" width="75.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="75.7109375" customWidth="1"/>
   </cols>
@@ -1329,7 +1255,7 @@
         <v>45</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="195" x14ac:dyDescent="0.25">
@@ -1352,7 +1278,7 @@
         <v>42</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="210" x14ac:dyDescent="0.25">
@@ -1375,7 +1301,7 @@
         <v>40</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1390,142 +1316,125 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F9C94FF-7882-493D-A7ED-509C78885EFA}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="5" width="26.28515625" customWidth="1"/>
-    <col min="6" max="6" width="31.5703125" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16" style="1" customWidth="1"/>
-    <col min="11" max="11" width="98.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16" style="1" customWidth="1"/>
+    <col min="9" max="9" width="98.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="16" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="16" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="E3" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="10">
+        <v>1</v>
+      </c>
+      <c r="H3" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" s="8">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="G3" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I3" s="10">
-        <v>1</v>
-      </c>
-      <c r="J3" s="10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="8">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="5"/>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{2BD1E75E-64EA-48A1-9E9B-B6E599E2ACB5}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{182E2115-1FB4-4931-99A3-1E5C126E1DD3}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update DefinitionInformation table documentation
</commit_message>
<xml_diff>
--- a/DefinitionInformationTable.xlsx
+++ b/DefinitionInformationTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TJB0303\LocalSave\R\GitHub\syndrome-definition-evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AAA4F4-0D3D-4195-9E45-BFB7AF0DAEEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDC6D5B-77D7-495B-8948-CF0407FCE486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D30C9C86-3D98-4204-9FB5-C398A54A23E4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{D30C9C86-3D98-4204-9FB5-C398A54A23E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="5" r:id="rId1"/>
@@ -224,35 +224,6 @@
     <t>Lauren Draftz</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">[Stratified random sample? </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(TRUE/FALSE)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>]</t>
-    </r>
-  </si>
-  <si>
-    <t>[Stratified random sample variable.]</t>
-  </si>
-  <si>
     <t>[Enter the fields that you want to use to explore in more detail. For each field listed below, you will see a "Top 5" chart showing the top 5 most frequently occuring free-text terms in that field. You must use the name as listed in the NSSP Data Dictionary "ESSENCE API and Data Details" tab under the "Data Details Web Display Name" column</t>
   </si>
   <si>
@@ -351,7 +322,275 @@
     </r>
   </si>
   <si>
+    <t>CCDDCategory_flat</t>
+  </si>
+  <si>
+    <t>Category_flat</t>
+  </si>
+  <si>
+    <t>Subcategory_flat</t>
+  </si>
+  <si>
+    <t>Procedure_Combo</t>
+  </si>
+  <si>
+    <t>DDParsed</t>
+  </si>
+  <si>
+    <t>ValidationReview</t>
+  </si>
+  <si>
+    <t>Year, Month</t>
+  </si>
+  <si>
     <t>proportion</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[Include Validation Review.]
+If </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TRUE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> edit "ValidationReviewInformation" sheet, if </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FALSE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do not edit "ValidationReviewInformation". </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3 recommended options for a Review Scale:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- 0-1 (0: False Positive | 1: True Positive); </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Default</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- 1-3 (1: Unlikely | 2:  Uncertain | 3: Likely) 
+- 1-5 (1: Very Unlikely, 2: Unlikely | 3: Uncertain | 4: Likely, 5: Very Likely)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>You may also specify a custom scale using ReviewScaleLow and ReviewScaleHigh:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Even length of numbers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ex:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1 to 6), an equal number of ratings will be assigned to "True Positive" and "False Positive" (</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ex:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1,2,3: False Positive | 4,5,6: True Positive).
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Odd length of numbers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ex:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1 to 7), the median will be assigned to "Uncertain" and an equal number of ratings will subsequently be assigned to "True Positive" and "False Positive" (</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ex:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1,2,3: False Positive | 4: Uncertain | 5,6,7: True Positive).</t>
+    </r>
   </si>
   <si>
     <r>
@@ -421,10 +660,35 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> decimal from 0 to 1 (ex: 0.4)</t>
-    </r>
-  </si>
-  <si>
+      <t xml:space="preserve"> decimal from 0 to 1 (</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ex:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 0.4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[Stratified random sample variable.]
+</t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -434,18 +698,38 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Note:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Here's 3 recommend options for a Review Scale. You may specify a new scale with ReviewScaleLow/High as well if you want. 
-- 0-1 (0: False Positive | 1: True Positive); </t>
+      <t xml:space="preserve">Options: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>single or in combination</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
     </r>
     <r>
       <rPr>
@@ -456,46 +740,24 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Default</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">
-- 1-3 (1: Unlikely | 2:  Uncertain | 3: Likely) 
-- 1-5 (1: Very Unlikely, 2: Unlikely | 3: Uncertain | 4: Likely, 5: Very Likely)</t>
-    </r>
-  </si>
-  <si>
-    <t>CCDDCategory_flat</t>
-  </si>
-  <si>
-    <t>Category_flat</t>
-  </si>
-  <si>
-    <t>Subcategory_flat</t>
-  </si>
-  <si>
-    <t>Procedure_Combo</t>
-  </si>
-  <si>
-    <t>DDParsed</t>
-  </si>
-  <si>
-    <t>Weekday, Month</t>
-  </si>
-  <si>
-    <t>ValidationReview</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">[Include Validation Review Validation.]
-If </t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Year, Month, Week, Weekday</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[Stratified random sample?
+</t>
     </r>
     <r>
       <rPr>
@@ -506,38 +768,19 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>TRUE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> edit "ValidationReviewInformation" sheet, if </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>FALSE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> do not edit "ValidationReviewInformation". </t>
+      <t>Options:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+- TRUE
+- FALSE</t>
     </r>
   </si>
 </sst>
@@ -545,7 +788,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -563,6 +806,31 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -989,10 +1257,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4B277CF-9876-4850-BAAE-A2FD71D015E1}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,7 +1293,7 @@
         <v>27</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -1048,7 +1316,7 @@
         <v>14</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1056,13 +1324,13 @@
         <v>30</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E3" s="6">
         <v>44256</v>
@@ -1087,8 +1355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A5C921F-19C2-4CBC-9726-8946A726EC05}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,7 +1366,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>34</v>
@@ -1117,7 +1385,7 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1125,7 +1393,7 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1133,7 +1401,7 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1141,7 +1409,7 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1149,7 +1417,7 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1177,7 +1445,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1255,7 +1523,7 @@
         <v>45</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="195" x14ac:dyDescent="0.25">
@@ -1278,7 +1546,7 @@
         <v>42</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="210" x14ac:dyDescent="0.25">
@@ -1301,7 +1569,7 @@
         <v>40</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1320,23 +1588,23 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
     <col min="4" max="4" width="31.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="16" style="1" customWidth="1"/>
-    <col min="9" max="9" width="98.85546875" customWidth="1"/>
+    <col min="9" max="9" width="103.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="16" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="16" customFormat="1" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>57</v>
       </c>
@@ -1344,16 +1612,16 @@
         <v>28</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="G1" s="15" t="s">
         <v>51</v>
@@ -1362,7 +1630,7 @@
         <v>52</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1373,10 +1641,10 @@
         <v>59</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E2" s="19" t="s">
         <v>53</v>
@@ -1399,7 +1667,7 @@
         <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D3" s="9">
         <v>0.25</v>
@@ -1408,7 +1676,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G3" s="10">
         <v>1</v>

</xml_diff>

<commit_message>
Set Excel Table defaults
</commit_message>
<xml_diff>
--- a/DefinitionInformationTable.xlsx
+++ b/DefinitionInformationTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TJB0303\LocalSave\R\GitHub\syndrome-definition-evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3942AA-5E4E-4538-B174-51EE4827A639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7057F0CE-CA5D-400C-9743-B6BCBCB94F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D30C9C86-3D98-4204-9FB5-C398A54A23E4}"/>
   </bookViews>
@@ -242,77 +242,6 @@
     <t>SampleValue</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">[Review sample metric. ]
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Options:
--</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (for number of records)
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>proportion</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (% of records)</t>
-    </r>
-  </si>
-  <si>
     <t>CCDDCategory_flat</t>
   </si>
   <si>
@@ -806,7 +735,78 @@
     </r>
   </si>
   <si>
-    <t>n</t>
+    <r>
+      <t xml:space="preserve">[Review sample metric. ]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Options:
+-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (for number of records)
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>proportion</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (% of records)</t>
+    </r>
+  </si>
+  <si>
+    <t>number</t>
   </si>
 </sst>
 </file>
@@ -1319,7 +1319,7 @@
         <v>27</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1342,7 +1342,7 @@
         <v>14</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1359,10 +1359,10 @@
         <v>63</v>
       </c>
       <c r="E3" s="4">
-        <v>44331</v>
+        <v>44986</v>
       </c>
       <c r="F3" s="4">
-        <v>44348</v>
+        <v>45078</v>
       </c>
       <c r="G3" s="6" t="b">
         <v>1</v>
@@ -1412,7 +1412,7 @@
         <v>25</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1420,7 +1420,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1428,7 +1428,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1436,7 +1436,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1444,7 +1444,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1613,9 +1613,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F9C94FF-7882-493D-A7ED-509C78885EFA}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1633,22 +1633,22 @@
   <sheetData>
     <row r="1" spans="1:9" s="11" customFormat="1" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>80</v>
-      </c>
       <c r="C1" s="16" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="D1" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>76</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>77</v>
       </c>
       <c r="G1" s="23" t="s">
         <v>51</v>
@@ -1657,7 +1657,7 @@
         <v>52</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1704,7 +1704,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G3" s="8">
         <v>1</v>
@@ -1718,7 +1718,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" s="19"/>
     </row>

</xml_diff>

<commit_message>
Update DefinitionInformationTable to allow for selection of dedup_dx()
</commit_message>
<xml_diff>
--- a/DefinitionInformationTable.xlsx
+++ b/DefinitionInformationTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TJB0303\LocalSave\R\GitHub\syndrome-definition-evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7057F0CE-CA5D-400C-9743-B6BCBCB94F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65966A5A-63D0-4ECF-BBC2-8059BD324278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D30C9C86-3D98-4204-9FB5-C398A54A23E4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{D30C9C86-3D98-4204-9FB5-C398A54A23E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="87">
   <si>
     <t>Syndrome</t>
   </si>
@@ -807,6 +807,64 @@
   </si>
   <si>
     <t>number</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[Deduplicate Discharge Diagnoses]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Options:
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">TRUE/FALSE
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Applies to:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- DischargeDiagnosis
+- Diagnosis_Combo
+- DDParsed
+- CCDD
+- CCDDParsed</t>
+    </r>
+  </si>
+  <si>
+    <t>DeduplicateDDx</t>
   </si>
 </sst>
 </file>
@@ -985,9 +1043,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1025,7 +1083,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1131,7 +1189,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1273,7 +1331,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1283,7 +1341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4B277CF-9876-4850-BAAE-A2FD71D015E1}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
@@ -1611,27 +1669,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F9C94FF-7882-493D-A7ED-509C78885EFA}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" style="6" customWidth="1"/>
     <col min="2" max="2" width="15.140625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="31.5703125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="17" style="5" customWidth="1"/>
-    <col min="6" max="6" width="33.7109375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="16" style="5" customWidth="1"/>
-    <col min="9" max="9" width="103.140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="17" style="5" customWidth="1"/>
+    <col min="7" max="7" width="33.7109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="16" style="5" customWidth="1"/>
+    <col min="10" max="10" width="103.140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="11" customFormat="1" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="11" customFormat="1" ht="185.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>78</v>
       </c>
@@ -1639,28 +1698,31 @@
         <v>79</v>
       </c>
       <c r="C1" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="E1" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="H1" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="I1" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="J1" s="16" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>57</v>
       </c>
@@ -1668,59 +1730,65 @@
         <v>58</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="E2" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="F2" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="G2" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="H2" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="I2" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="18"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="18"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="7">
+      <c r="E3" s="7">
         <v>100</v>
       </c>
-      <c r="E3" s="5" t="b">
+      <c r="F3" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="8">
+      <c r="H3" s="8">
         <v>1</v>
       </c>
-      <c r="H3" s="8">
+      <c r="I3" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add variables to pull (AgeGroup) for demo table
</commit_message>
<xml_diff>
--- a/DefinitionInformationTable.xlsx
+++ b/DefinitionInformationTable.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TJB0303\LocalSave\R\GitHub\syndrome-definition-evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E454BD54-FCB4-43F2-9754-C471ABCEE819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30008613-FD9B-4907-B10B-C10AB8F48258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{D30C9C86-3D98-4204-9FB5-C398A54A23E4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{D30C9C86-3D98-4204-9FB5-C398A54A23E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="5" r:id="rId1"/>
-    <sheet name="AppliedFields" sheetId="6" r:id="rId2"/>
+    <sheet name="SelectFields" sheetId="9" r:id="rId2"/>
     <sheet name="DefinitionInformation" sheetId="1" r:id="rId3"/>
     <sheet name="ValidationReviewInformation" sheetId="7" r:id="rId4"/>
   </sheets>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="120">
   <si>
     <t>Syndrome</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Structure</t>
   </si>
   <si>
-    <t>Chief Complaint History, Discharge Diagnosis or Admit Reason Combo</t>
-  </si>
-  <si>
     <t>[Syndrome name from ESSENCE]</t>
   </si>
   <si>
@@ -89,12 +86,6 @@
     <t>[The jurisdiction you are applying this query to.]</t>
   </si>
   <si>
-    <t>Field</t>
-  </si>
-  <si>
-    <t>DischargeDiagnosis</t>
-  </si>
-  <si>
     <t>Diagnosis_Combo</t>
   </si>
   <si>
@@ -137,12 +128,6 @@
     <t>[Your organization name.]</t>
   </si>
   <si>
-    <t>DoNotUse</t>
-  </si>
-  <si>
-    <t>[For any fields you do not want to see a "Top 5 Terms" chart, cut and paste the name into this column so it will be excluded. If a field appears here, it will not be included.]</t>
-  </si>
-  <si>
     <t>[Abbreviated name for the definition. This is up to you as the author, so choose something that will make sense and be recogniable to you in your report.]</t>
   </si>
   <si>
@@ -213,9 +198,6 @@
   </si>
   <si>
     <t>ReviewerName</t>
-  </si>
-  <si>
-    <t>[Enter the fields that you want to use to explore in more detail. For each field listed below, you will see a "Top 5" chart showing the top 5 most frequently occuring free-text terms in that field. You must use the name as listed in the NSSP Data Dictionary "ESSENCE API and Data Details" tab under the "Data Details Web Display Name" column</t>
   </si>
   <si>
     <t>https://essence.syndromicsurveillance.org/nssp_essence/api/dataDetails/csv?geography=wa&amp;datasource=va_hosp&amp;startDate=19Oct2023&amp;medicalGroupingSystem=essencesyndromes&amp;userId=4714&amp;endDate=20Oct2023&amp;percentParam=noPercent&amp;hospFacilityType=emergency%20care&amp;aqtTarget=DataDetails&amp;ccddCategory=cdc%20influenza%20dd%20v1&amp;geographySystem=hospitalstate&amp;detector=probrepswitch&amp;timeResolution=daily&amp;hasBeenE=1&amp;refValues=true</t>
@@ -865,6 +847,123 @@
   </si>
   <si>
     <t>DeduplicateDDx</t>
+  </si>
+  <si>
+    <t>C_BioSense_ID</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>CCDDParsed</t>
+  </si>
+  <si>
+    <t>Procedure_Code</t>
+  </si>
+  <si>
+    <t>Race_flat</t>
+  </si>
+  <si>
+    <t>Ethnicity_flat</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>HospitalRegion</t>
+  </si>
+  <si>
+    <t>MinutesFromVisitToDischarge</t>
+  </si>
+  <si>
+    <t>HasBeenE</t>
+  </si>
+  <si>
+    <t>HasBeenI</t>
+  </si>
+  <si>
+    <t>C_Death</t>
+  </si>
+  <si>
+    <t>DispositionCategory</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>ESSENCEfields</t>
+  </si>
+  <si>
+    <t>[Update this column to Yes if you would like to have the field included in the outputs for manual review.]</t>
+  </si>
+  <si>
+    <t>[Update this column to Yes if you would like to have the field included in the "Top 5 Term" text analysis output.]</t>
+  </si>
+  <si>
+    <t>[This list contains a common set of fields from the data details results that may be helpful in evaluating the results from a syndrome definition. To add additional fields, consult the "ESSENCE API and Data Details" tab of the NSSP Data Dictionary.]</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Not eligible for free text analysis</t>
+  </si>
+  <si>
+    <t>[Do not edit this column.]</t>
+  </si>
+  <si>
+    <t>Redundancy: ChiefComplaintOrig is found in ChiefComplaintUpdates</t>
+  </si>
+  <si>
+    <t>Redundancy: ChiefComplaintParsed is found in both CCDD and CCDDParsed.</t>
+  </si>
+  <si>
+    <t>Redundancy: DischargeDiagnosisParsed is found in CCDDParsed</t>
+  </si>
+  <si>
+    <t>Redundancy: Recommended to use CCDDParsed because of the standardization of the discharge diagnoses, CC segment is the same</t>
+  </si>
+  <si>
+    <t>ClinicalImpression</t>
+  </si>
+  <si>
+    <t>Initial_Pulse_Oximetry_Calc</t>
+  </si>
+  <si>
+    <t>Initial_Temp_Calc</t>
+  </si>
+  <si>
+    <t>IncludeForValidationReview</t>
+  </si>
+  <si>
+    <t>IncludeForTextAnalysis</t>
+  </si>
+  <si>
+    <t>c_race</t>
+  </si>
+  <si>
+    <t>c_ethnicity</t>
+  </si>
+  <si>
+    <t>Chief Complaint History, Discharge Diagnosis, or Admit Reason Combo</t>
+  </si>
+  <si>
+    <t>DischargeDiagnosis</t>
+  </si>
+  <si>
+    <t>Redundancy: DischargeDiagnosis is found in CCDDParsed</t>
+  </si>
+  <si>
+    <t>AgeGroup</t>
   </si>
 </sst>
 </file>
@@ -1029,7 +1128,28 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1344,7 +1464,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1359,62 +1479,62 @@
   <sheetData>
     <row r="1" spans="1:7" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E2" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>14</v>
-      </c>
       <c r="G2" s="18" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E3" s="4">
         <v>44986</v>
@@ -1436,91 +1556,499 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A5C921F-19C2-4CBC-9726-8946A726EC05}">
-  <dimension ref="A1:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C00C859-E9BD-4CEE-A4ED-0B7D92D4D6F1}">
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" style="6" customWidth="1"/>
+    <col min="1" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="133" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" t="s">
+        <v>97</v>
+      </c>
+      <c r="D27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="B33" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>24</v>
+      <c r="B34" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" t="s">
+        <v>96</v>
+      </c>
+      <c r="D34" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" t="s">
+        <v>96</v>
+      </c>
+      <c r="D36" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:C1048576">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1531,7 +2059,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1547,33 +2075,33 @@
     <row r="1" spans="1:7" s="11" customFormat="1" ht="86.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15"/>
       <c r="B1" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>1</v>
@@ -1585,76 +2113,76 @@
         <v>3</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="225" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>4</v>
+        <v>116</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="210" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>4</v>
+        <v>116</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1671,7 +2199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F9C94FF-7882-493D-A7ED-509C78885EFA}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
@@ -1692,63 +2220,63 @@
   <sheetData>
     <row r="1" spans="1:10" s="11" customFormat="1" ht="185.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>85</v>
-      </c>
       <c r="D1" s="16" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="H1" s="23" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="J2" s="18"/>
     </row>
@@ -1757,13 +2285,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C3" s="6" t="b">
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E3" s="7">
         <v>100</v>
@@ -1772,7 +2300,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H3" s="8">
         <v>1</v>
@@ -1786,7 +2314,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D4" s="19"/>
     </row>

</xml_diff>